<commit_message>
Update Informazioni progetto IS.xlsx
</commit_message>
<xml_diff>
--- a/Informazioni progetto IS.xlsx
+++ b/Informazioni progetto IS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaella/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaella/Documents/BestToWatch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DAE9BD-6E47-4F44-ACAD-76B404FDCC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC6CC3E-FE3C-E443-8EB6-370EC60ABBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="progetto" sheetId="2" r:id="rId1"/>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Descrizione Sintetica</t>
-  </si>
-  <si>
-    <t>Best to watch</t>
   </si>
   <si>
     <t xml:space="preserve">Piattaforma di streaming video </t>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>https://github.com/Tsunami909/BestToWatch.git</t>
+  </si>
+  <si>
+    <t>Best To Watch</t>
   </si>
 </sst>
 </file>
@@ -1354,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1382,13 +1382,13 @@
     </row>
     <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1465,7 +1465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1478,61 +1480,61 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -3257,6 +3259,9 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="A2:A4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>